<commit_message>
Corrección de Informes mensuales
</commit_message>
<xml_diff>
--- a/Marzo/Informes/8. RE-M-IN-74 Formato Informe mensual yo periódico de estímulos académicos LUIS ENRIQUE GUERRERO.xlsx
+++ b/Marzo/Informes/8. RE-M-IN-74 Formato Informe mensual yo periódico de estímulos académicos LUIS ENRIQUE GUERRERO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\ESAP\Monitorias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\ESAP\Monitorias\tendencias de Administración Pública\Marzo\Informes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC55935-4FDA-4659-B1D5-A63549F33D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61255B46-EE6D-47D3-A102-37B3BA3EB605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="405" windowWidth="19200" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informe Mensual RE-M-IN-74" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="176">
   <si>
     <t xml:space="preserve">Dependencia: </t>
   </si>
@@ -576,9 +576,6 @@
     <t>Tipo de vinculación</t>
   </si>
   <si>
-    <t>DD/MM/AA</t>
-  </si>
-  <si>
     <t>Del 06 de marzo al 05 de abril</t>
   </si>
   <si>
@@ -925,6 +922,18 @@
   </si>
   <si>
     <t>458070021381</t>
+  </si>
+  <si>
+    <t>Por la cual se otorga Estímulo Académico en la modalidad de Monitor a Diez (10)Estudiantes de la Sede Central de la Escuela Superior de Administración Pública, 2023</t>
+  </si>
+  <si>
+    <t>Investigación aplicada: Innovación y tendencias de la administración pública</t>
+  </si>
+  <si>
+    <t>Sede Central Bogotá</t>
+  </si>
+  <si>
+    <t>Del 08 de marzo al 01 de abril</t>
   </si>
 </sst>
 </file>
@@ -2584,6 +2593,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="37" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2795,10 +2808,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="37" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -17884,8 +17893,8 @@
   </sheetPr>
   <dimension ref="A1:ES99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="113" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:K18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -18087,7 +18096,9 @@
       </c>
       <c r="E7" s="182"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="216"/>
+      <c r="G7" s="216" t="s">
+        <v>112</v>
+      </c>
       <c r="H7" s="217"/>
       <c r="I7" s="218"/>
       <c r="J7" s="52"/>
@@ -18095,14 +18106,18 @@
         <v>16</v>
       </c>
       <c r="L7" s="52"/>
-      <c r="M7" s="211"/>
+      <c r="M7" s="211">
+        <v>1</v>
+      </c>
       <c r="N7" s="52"/>
       <c r="O7" s="52"/>
       <c r="P7" s="182" t="s">
         <v>15</v>
       </c>
       <c r="Q7" s="52"/>
-      <c r="R7" s="211"/>
+      <c r="R7" s="211">
+        <v>10</v>
+      </c>
       <c r="S7" s="52"/>
       <c r="T7" s="181" t="s">
         <v>1</v>
@@ -18144,9 +18159,13 @@
       <c r="S8" s="10"/>
       <c r="T8" s="181"/>
       <c r="U8" s="13"/>
-      <c r="V8" s="57"/>
+      <c r="V8" s="57">
+        <v>29</v>
+      </c>
       <c r="W8" s="35"/>
-      <c r="X8" s="57"/>
+      <c r="X8" s="57" t="s">
+        <v>40</v>
+      </c>
       <c r="Y8" s="35"/>
       <c r="Z8" s="77">
         <v>2023</v>
@@ -18294,7 +18313,9 @@
         <v>3</v>
       </c>
       <c r="H13" s="49"/>
-      <c r="I13" s="195"/>
+      <c r="I13" s="195">
+        <v>312</v>
+      </c>
       <c r="J13" s="196"/>
       <c r="K13" s="196"/>
       <c r="L13" s="197"/>
@@ -18313,9 +18334,13 @@
       <c r="S13" s="172"/>
       <c r="T13" s="172"/>
       <c r="U13" s="49"/>
-      <c r="V13" s="46"/>
+      <c r="V13" s="46">
+        <v>8</v>
+      </c>
       <c r="W13" s="26"/>
-      <c r="X13" s="46"/>
+      <c r="X13" s="46" t="s">
+        <v>40</v>
+      </c>
       <c r="Y13" s="26"/>
       <c r="Z13" s="38">
         <v>2023</v>
@@ -18365,16 +18390,16 @@
         <v>91</v>
       </c>
       <c r="H15" s="29"/>
-      <c r="I15" s="236" t="s">
-        <v>155</v>
-      </c>
-      <c r="J15" s="237"/>
-      <c r="K15" s="237"/>
-      <c r="L15" s="237"/>
-      <c r="M15" s="237"/>
-      <c r="N15" s="237"/>
-      <c r="O15" s="237"/>
-      <c r="P15" s="238"/>
+      <c r="I15" s="237">
+        <v>44993</v>
+      </c>
+      <c r="J15" s="238"/>
+      <c r="K15" s="238"/>
+      <c r="L15" s="238"/>
+      <c r="M15" s="238"/>
+      <c r="N15" s="238"/>
+      <c r="O15" s="238"/>
+      <c r="P15" s="239"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="172" t="s">
         <v>4</v>
@@ -18382,9 +18407,13 @@
       <c r="S15" s="172"/>
       <c r="T15" s="172"/>
       <c r="U15" s="49"/>
-      <c r="V15" s="46"/>
+      <c r="V15" s="46">
+        <v>30</v>
+      </c>
       <c r="W15" s="26"/>
-      <c r="X15" s="46"/>
+      <c r="X15" s="46" t="s">
+        <v>48</v>
+      </c>
       <c r="Y15" s="26"/>
       <c r="Z15" s="38">
         <v>2023</v>
@@ -18405,32 +18434,36 @@
         <v>51</v>
       </c>
       <c r="H16" s="49"/>
-      <c r="I16" s="234">
+      <c r="I16" s="235">
         <v>73023</v>
       </c>
-      <c r="J16" s="234"/>
+      <c r="J16" s="235"/>
       <c r="K16" s="45" t="s">
         <v>5</v>
       </c>
       <c r="L16" s="49"/>
-      <c r="M16" s="235" t="s">
-        <v>155</v>
-      </c>
-      <c r="N16" s="235"/>
-      <c r="O16" s="235"/>
-      <c r="P16" s="235"/>
+      <c r="M16" s="236">
+        <v>44986</v>
+      </c>
+      <c r="N16" s="236"/>
+      <c r="O16" s="236"/>
+      <c r="P16" s="236"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="S16" s="7"/>
-      <c r="T16" s="124"/>
+      <c r="T16" s="124">
+        <v>9</v>
+      </c>
       <c r="U16" s="45"/>
       <c r="V16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="W16" s="7"/>
-      <c r="X16" s="124"/>
+      <c r="X16" s="124">
+        <v>23</v>
+      </c>
       <c r="Y16" s="45"/>
       <c r="Z16" s="45" t="s">
         <v>103</v>
@@ -18456,18 +18489,20 @@
         <v>8</v>
       </c>
       <c r="L17" s="49"/>
-      <c r="M17" s="239" t="s">
-        <v>155</v>
-      </c>
-      <c r="N17" s="239"/>
-      <c r="O17" s="239"/>
-      <c r="P17" s="239"/>
+      <c r="M17" s="240">
+        <v>44993</v>
+      </c>
+      <c r="N17" s="240"/>
+      <c r="O17" s="240"/>
+      <c r="P17" s="240"/>
       <c r="Q17" s="45"/>
       <c r="R17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="S17" s="7"/>
-      <c r="T17" s="198"/>
+      <c r="T17" s="198" t="s">
+        <v>175</v>
+      </c>
       <c r="U17" s="198"/>
       <c r="V17" s="198"/>
       <c r="W17" s="198"/>
@@ -18526,12 +18561,10 @@
         <v>8</v>
       </c>
       <c r="L19" s="49"/>
-      <c r="M19" s="240" t="s">
-        <v>155</v>
-      </c>
-      <c r="N19" s="240"/>
-      <c r="O19" s="240"/>
-      <c r="P19" s="240"/>
+      <c r="M19" s="241"/>
+      <c r="N19" s="241"/>
+      <c r="O19" s="241"/>
+      <c r="P19" s="241"/>
       <c r="Q19" s="49"/>
       <c r="R19" s="49"/>
       <c r="S19" s="49"/>
@@ -18614,7 +18647,9 @@
       </c>
       <c r="E22" s="166"/>
       <c r="F22" s="167"/>
-      <c r="G22" s="204"/>
+      <c r="G22" s="204" t="s">
+        <v>172</v>
+      </c>
       <c r="H22" s="205"/>
       <c r="I22" s="205"/>
       <c r="J22" s="205"/>
@@ -18752,7 +18787,9 @@
       <c r="E27" s="193"/>
       <c r="F27" s="193"/>
       <c r="G27" s="193"/>
-      <c r="H27" s="159"/>
+      <c r="H27" s="159" t="s">
+        <v>173</v>
+      </c>
       <c r="I27" s="159"/>
       <c r="J27" s="159"/>
       <c r="K27" s="159"/>
@@ -18814,7 +18851,9 @@
       <c r="E29" s="186"/>
       <c r="F29" s="186"/>
       <c r="G29" s="186"/>
-      <c r="H29" s="160"/>
+      <c r="H29" s="160" t="s">
+        <v>174</v>
+      </c>
       <c r="I29" s="160"/>
       <c r="J29" s="160"/>
       <c r="K29" s="160"/>
@@ -18962,7 +19001,7 @@
       <c r="E34" s="172"/>
       <c r="F34" s="49"/>
       <c r="G34" s="173" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H34" s="174"/>
       <c r="I34" s="174"/>
@@ -19042,11 +19081,11 @@
         <v>3</v>
       </c>
       <c r="Q36" s="45"/>
-      <c r="R36" s="231">
+      <c r="R36" s="232">
         <v>98394126</v>
       </c>
-      <c r="S36" s="232"/>
-      <c r="T36" s="233"/>
+      <c r="S36" s="233"/>
+      <c r="T36" s="234"/>
       <c r="X36" s="45"/>
       <c r="Y36" s="45"/>
       <c r="Z36" s="85"/>
@@ -19063,22 +19102,22 @@
       <c r="E37" s="172"/>
       <c r="F37" s="49"/>
       <c r="G37" s="185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H37" s="185"/>
       <c r="I37" s="185"/>
       <c r="J37" s="185"/>
       <c r="K37" s="185"/>
       <c r="L37" s="18"/>
-      <c r="M37" s="230" t="s">
+      <c r="M37" s="231" t="s">
         <v>98</v>
       </c>
-      <c r="N37" s="230"/>
-      <c r="O37" s="230"/>
-      <c r="P37" s="230"/>
+      <c r="N37" s="231"/>
+      <c r="O37" s="231"/>
+      <c r="P37" s="231"/>
       <c r="Q37" s="18"/>
-      <c r="R37" s="296" t="s">
-        <v>171</v>
+      <c r="R37" s="230" t="s">
+        <v>170</v>
       </c>
       <c r="S37" s="185"/>
       <c r="T37" s="185"/>
@@ -19130,13 +19169,13 @@
       </c>
       <c r="E39" s="172"/>
       <c r="F39" s="49"/>
-      <c r="G39" s="243">
+      <c r="G39" s="244">
         <v>3208172936</v>
       </c>
-      <c r="H39" s="243"/>
-      <c r="I39" s="243"/>
-      <c r="J39" s="243"/>
-      <c r="K39" s="243"/>
+      <c r="H39" s="244"/>
+      <c r="I39" s="244"/>
+      <c r="J39" s="244"/>
+      <c r="K39" s="244"/>
       <c r="M39" s="7" t="s">
         <v>37</v>
       </c>
@@ -19204,7 +19243,7 @@
         <v>3</v>
       </c>
       <c r="N41" s="183" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O41" s="183"/>
       <c r="P41" s="183"/>
@@ -19430,9 +19469,9 @@
         <v>3</v>
       </c>
       <c r="Q48" s="45"/>
-      <c r="R48" s="231"/>
-      <c r="S48" s="232"/>
-      <c r="T48" s="233"/>
+      <c r="R48" s="232"/>
+      <c r="S48" s="233"/>
+      <c r="T48" s="234"/>
       <c r="X48" s="45"/>
       <c r="Y48" s="45"/>
       <c r="Z48" s="85"/>
@@ -19454,12 +19493,12 @@
       <c r="J49" s="185"/>
       <c r="K49" s="185"/>
       <c r="L49" s="18"/>
-      <c r="M49" s="230" t="s">
+      <c r="M49" s="231" t="s">
         <v>98</v>
       </c>
-      <c r="N49" s="230"/>
-      <c r="O49" s="230"/>
-      <c r="P49" s="230"/>
+      <c r="N49" s="231"/>
+      <c r="O49" s="231"/>
+      <c r="P49" s="231"/>
       <c r="Q49" s="18"/>
       <c r="R49" s="185"/>
       <c r="S49" s="185"/>
@@ -19512,11 +19551,11 @@
       </c>
       <c r="E51" s="172"/>
       <c r="F51" s="49"/>
-      <c r="G51" s="243"/>
-      <c r="H51" s="243"/>
-      <c r="I51" s="243"/>
-      <c r="J51" s="243"/>
-      <c r="K51" s="243"/>
+      <c r="G51" s="244"/>
+      <c r="H51" s="244"/>
+      <c r="I51" s="244"/>
+      <c r="J51" s="244"/>
+      <c r="K51" s="244"/>
       <c r="M51" s="7" t="s">
         <v>37</v>
       </c>
@@ -19724,8 +19763,8 @@
         <v>74</v>
       </c>
       <c r="I58" s="190">
-        <f>1250000*8</f>
-        <v>10000000</v>
+        <f>12208333</f>
+        <v>12208333</v>
       </c>
       <c r="J58" s="190"/>
       <c r="K58" s="190"/>
@@ -19784,7 +19823,7 @@
       </c>
       <c r="I60" s="191">
         <f>+I58</f>
-        <v>10000000</v>
+        <v>12208333</v>
       </c>
       <c r="J60" s="191"/>
       <c r="K60" s="191"/>
@@ -19930,21 +19969,21 @@
       <c r="A65" s="6"/>
       <c r="B65" s="97"/>
       <c r="G65" s="157">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="H65" s="47"/>
       <c r="I65" s="157">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="J65" s="47">
         <v>1250000</v>
       </c>
       <c r="K65" s="158">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="L65" s="47"/>
       <c r="M65" s="158">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="N65" s="47"/>
       <c r="O65" s="47"/>
@@ -20029,15 +20068,15 @@
       <c r="A68" s="6"/>
       <c r="B68" s="97"/>
       <c r="G68" s="157">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="H68" s="47"/>
       <c r="I68" s="157">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="J68" s="47"/>
       <c r="K68" s="158">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="L68" s="47"/>
       <c r="M68" s="158">
@@ -20219,7 +20258,7 @@
       <c r="H74" s="50"/>
       <c r="I74" s="168">
         <f>G65+I65+K65+M65+G68+M68+G71+I71+K71+M71+I68+K68</f>
-        <v>8750000</v>
+        <v>0</v>
       </c>
       <c r="J74" s="168"/>
       <c r="K74" s="168"/>
@@ -20253,7 +20292,7 @@
       <c r="G75" s="50"/>
       <c r="H75" s="50"/>
       <c r="I75" s="188">
-        <v>1250000</v>
+        <v>958333</v>
       </c>
       <c r="J75" s="188"/>
       <c r="K75" s="188"/>
@@ -20288,7 +20327,7 @@
       <c r="H76" s="50"/>
       <c r="I76" s="168">
         <f>(I60)-(I74+I75)</f>
-        <v>0</v>
+        <v>11250000</v>
       </c>
       <c r="J76" s="168"/>
       <c r="K76" s="168"/>
@@ -20343,32 +20382,32 @@
     </row>
     <row r="78" spans="1:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="97"/>
-      <c r="C78" s="260" t="s">
+      <c r="C78" s="261" t="s">
         <v>100</v>
       </c>
-      <c r="D78" s="261"/>
-      <c r="E78" s="261"/>
-      <c r="F78" s="244"/>
-      <c r="G78" s="244"/>
-      <c r="H78" s="244"/>
-      <c r="I78" s="244"/>
-      <c r="J78" s="244"/>
-      <c r="K78" s="244"/>
-      <c r="L78" s="244"/>
-      <c r="M78" s="244"/>
-      <c r="N78" s="244"/>
-      <c r="O78" s="244"/>
-      <c r="P78" s="252" t="s">
+      <c r="D78" s="262"/>
+      <c r="E78" s="262"/>
+      <c r="F78" s="245"/>
+      <c r="G78" s="245"/>
+      <c r="H78" s="245"/>
+      <c r="I78" s="245"/>
+      <c r="J78" s="245"/>
+      <c r="K78" s="245"/>
+      <c r="L78" s="245"/>
+      <c r="M78" s="245"/>
+      <c r="N78" s="245"/>
+      <c r="O78" s="245"/>
+      <c r="P78" s="253" t="s">
         <v>83</v>
       </c>
-      <c r="Q78" s="253"/>
-      <c r="R78" s="253"/>
-      <c r="S78" s="253"/>
-      <c r="T78" s="253"/>
-      <c r="U78" s="253"/>
-      <c r="V78" s="253"/>
-      <c r="W78" s="253"/>
-      <c r="X78" s="253"/>
+      <c r="Q78" s="254"/>
+      <c r="R78" s="254"/>
+      <c r="S78" s="254"/>
+      <c r="T78" s="254"/>
+      <c r="U78" s="254"/>
+      <c r="V78" s="254"/>
+      <c r="W78" s="254"/>
+      <c r="X78" s="254"/>
       <c r="Y78" s="7"/>
       <c r="Z78" s="7"/>
       <c r="AA78" s="114"/>
@@ -20377,20 +20416,20 @@
     </row>
     <row r="79" spans="1:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="97"/>
-      <c r="C79" s="262"/>
-      <c r="D79" s="263"/>
-      <c r="E79" s="263"/>
-      <c r="F79" s="244"/>
-      <c r="G79" s="244"/>
-      <c r="H79" s="244"/>
-      <c r="I79" s="244"/>
-      <c r="J79" s="244"/>
-      <c r="K79" s="244"/>
-      <c r="L79" s="244"/>
-      <c r="M79" s="244"/>
-      <c r="N79" s="244"/>
-      <c r="O79" s="244"/>
-      <c r="P79" s="251" t="s">
+      <c r="C79" s="263"/>
+      <c r="D79" s="264"/>
+      <c r="E79" s="264"/>
+      <c r="F79" s="245"/>
+      <c r="G79" s="245"/>
+      <c r="H79" s="245"/>
+      <c r="I79" s="245"/>
+      <c r="J79" s="245"/>
+      <c r="K79" s="245"/>
+      <c r="L79" s="245"/>
+      <c r="M79" s="245"/>
+      <c r="N79" s="245"/>
+      <c r="O79" s="245"/>
+      <c r="P79" s="252" t="s">
         <v>35</v>
       </c>
       <c r="Q79" s="200"/>
@@ -20409,20 +20448,20 @@
     </row>
     <row r="80" spans="1:29" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="97"/>
-      <c r="C80" s="264"/>
-      <c r="D80" s="265"/>
-      <c r="E80" s="265"/>
-      <c r="F80" s="244"/>
-      <c r="G80" s="244"/>
-      <c r="H80" s="244"/>
-      <c r="I80" s="244"/>
-      <c r="J80" s="244"/>
-      <c r="K80" s="244"/>
-      <c r="L80" s="244"/>
-      <c r="M80" s="244"/>
-      <c r="N80" s="244"/>
-      <c r="O80" s="244"/>
-      <c r="P80" s="251" t="s">
+      <c r="C80" s="265"/>
+      <c r="D80" s="266"/>
+      <c r="E80" s="266"/>
+      <c r="F80" s="245"/>
+      <c r="G80" s="245"/>
+      <c r="H80" s="245"/>
+      <c r="I80" s="245"/>
+      <c r="J80" s="245"/>
+      <c r="K80" s="245"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="245"/>
+      <c r="N80" s="245"/>
+      <c r="O80" s="245"/>
+      <c r="P80" s="252" t="s">
         <v>33</v>
       </c>
       <c r="Q80" s="200"/>
@@ -20441,62 +20480,62 @@
     </row>
     <row r="81" spans="2:29" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="97"/>
-      <c r="C81" s="241"/>
-      <c r="D81" s="242"/>
-      <c r="E81" s="242"/>
-      <c r="F81" s="242"/>
-      <c r="G81" s="242"/>
-      <c r="H81" s="242"/>
-      <c r="I81" s="242"/>
-      <c r="J81" s="242"/>
-      <c r="K81" s="242"/>
-      <c r="L81" s="242"/>
-      <c r="M81" s="242"/>
-      <c r="N81" s="242"/>
-      <c r="O81" s="242"/>
-      <c r="P81" s="242"/>
-      <c r="Q81" s="242"/>
-      <c r="R81" s="242"/>
-      <c r="S81" s="242"/>
-      <c r="T81" s="242"/>
-      <c r="U81" s="242"/>
-      <c r="V81" s="242"/>
-      <c r="W81" s="242"/>
-      <c r="X81" s="242"/>
-      <c r="Y81" s="242"/>
-      <c r="Z81" s="242"/>
+      <c r="C81" s="242"/>
+      <c r="D81" s="243"/>
+      <c r="E81" s="243"/>
+      <c r="F81" s="243"/>
+      <c r="G81" s="243"/>
+      <c r="H81" s="243"/>
+      <c r="I81" s="243"/>
+      <c r="J81" s="243"/>
+      <c r="K81" s="243"/>
+      <c r="L81" s="243"/>
+      <c r="M81" s="243"/>
+      <c r="N81" s="243"/>
+      <c r="O81" s="243"/>
+      <c r="P81" s="243"/>
+      <c r="Q81" s="243"/>
+      <c r="R81" s="243"/>
+      <c r="S81" s="243"/>
+      <c r="T81" s="243"/>
+      <c r="U81" s="243"/>
+      <c r="V81" s="243"/>
+      <c r="W81" s="243"/>
+      <c r="X81" s="243"/>
+      <c r="Y81" s="243"/>
+      <c r="Z81" s="243"/>
       <c r="AA81" s="99"/>
       <c r="AB81" s="134"/>
       <c r="AC81" s="2"/>
     </row>
     <row r="82" spans="2:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="97"/>
-      <c r="C82" s="260" t="s">
+      <c r="C82" s="261" t="s">
         <v>105</v>
       </c>
-      <c r="D82" s="261"/>
-      <c r="E82" s="261"/>
-      <c r="F82" s="291"/>
-      <c r="G82" s="292"/>
-      <c r="H82" s="292"/>
-      <c r="I82" s="292"/>
-      <c r="J82" s="292"/>
-      <c r="K82" s="292"/>
-      <c r="L82" s="292"/>
-      <c r="M82" s="292"/>
-      <c r="N82" s="292"/>
-      <c r="O82" s="292"/>
-      <c r="P82" s="252" t="s">
+      <c r="D82" s="262"/>
+      <c r="E82" s="262"/>
+      <c r="F82" s="292"/>
+      <c r="G82" s="293"/>
+      <c r="H82" s="293"/>
+      <c r="I82" s="293"/>
+      <c r="J82" s="293"/>
+      <c r="K82" s="293"/>
+      <c r="L82" s="293"/>
+      <c r="M82" s="293"/>
+      <c r="N82" s="293"/>
+      <c r="O82" s="293"/>
+      <c r="P82" s="253" t="s">
         <v>106</v>
       </c>
-      <c r="Q82" s="253"/>
-      <c r="R82" s="253"/>
-      <c r="S82" s="253"/>
-      <c r="T82" s="253"/>
-      <c r="U82" s="253"/>
-      <c r="V82" s="253"/>
-      <c r="W82" s="253"/>
-      <c r="X82" s="253"/>
+      <c r="Q82" s="254"/>
+      <c r="R82" s="254"/>
+      <c r="S82" s="254"/>
+      <c r="T82" s="254"/>
+      <c r="U82" s="254"/>
+      <c r="V82" s="254"/>
+      <c r="W82" s="254"/>
+      <c r="X82" s="254"/>
       <c r="Y82" s="7"/>
       <c r="Z82" s="7"/>
       <c r="AA82" s="114"/>
@@ -20505,20 +20544,20 @@
     </row>
     <row r="83" spans="2:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="97"/>
-      <c r="C83" s="262"/>
-      <c r="D83" s="263"/>
-      <c r="E83" s="263"/>
-      <c r="F83" s="292"/>
-      <c r="G83" s="292"/>
-      <c r="H83" s="292"/>
-      <c r="I83" s="292"/>
-      <c r="J83" s="292"/>
-      <c r="K83" s="292"/>
-      <c r="L83" s="292"/>
-      <c r="M83" s="292"/>
-      <c r="N83" s="292"/>
-      <c r="O83" s="292"/>
-      <c r="P83" s="251" t="s">
+      <c r="C83" s="263"/>
+      <c r="D83" s="264"/>
+      <c r="E83" s="264"/>
+      <c r="F83" s="293"/>
+      <c r="G83" s="293"/>
+      <c r="H83" s="293"/>
+      <c r="I83" s="293"/>
+      <c r="J83" s="293"/>
+      <c r="K83" s="293"/>
+      <c r="L83" s="293"/>
+      <c r="M83" s="293"/>
+      <c r="N83" s="293"/>
+      <c r="O83" s="293"/>
+      <c r="P83" s="252" t="s">
         <v>35</v>
       </c>
       <c r="Q83" s="200"/>
@@ -20537,20 +20576,20 @@
     </row>
     <row r="84" spans="2:29" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="97"/>
-      <c r="C84" s="264"/>
-      <c r="D84" s="265"/>
-      <c r="E84" s="265"/>
-      <c r="F84" s="292"/>
-      <c r="G84" s="292"/>
-      <c r="H84" s="292"/>
-      <c r="I84" s="292"/>
-      <c r="J84" s="292"/>
-      <c r="K84" s="292"/>
-      <c r="L84" s="292"/>
-      <c r="M84" s="292"/>
-      <c r="N84" s="292"/>
-      <c r="O84" s="292"/>
-      <c r="P84" s="251" t="s">
+      <c r="C84" s="265"/>
+      <c r="D84" s="266"/>
+      <c r="E84" s="266"/>
+      <c r="F84" s="293"/>
+      <c r="G84" s="293"/>
+      <c r="H84" s="293"/>
+      <c r="I84" s="293"/>
+      <c r="J84" s="293"/>
+      <c r="K84" s="293"/>
+      <c r="L84" s="293"/>
+      <c r="M84" s="293"/>
+      <c r="N84" s="293"/>
+      <c r="O84" s="293"/>
+      <c r="P84" s="252" t="s">
         <v>33</v>
       </c>
       <c r="Q84" s="200"/>
@@ -20600,17 +20639,17 @@
     <row r="86" spans="2:29" s="6" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="97"/>
       <c r="C86" s="7"/>
-      <c r="D86" s="286" t="s">
+      <c r="D86" s="287" t="s">
         <v>33</v>
       </c>
-      <c r="E86" s="286"/>
+      <c r="E86" s="287"/>
       <c r="F86" s="54"/>
-      <c r="G86" s="277"/>
-      <c r="H86" s="278"/>
-      <c r="I86" s="278"/>
-      <c r="J86" s="278"/>
-      <c r="K86" s="278"/>
-      <c r="L86" s="279"/>
+      <c r="G86" s="278"/>
+      <c r="H86" s="279"/>
+      <c r="I86" s="279"/>
+      <c r="J86" s="279"/>
+      <c r="K86" s="279"/>
+      <c r="L86" s="280"/>
       <c r="M86" s="7"/>
       <c r="N86" s="88"/>
       <c r="O86" s="88"/>
@@ -20632,29 +20671,29 @@
     <row r="87" spans="2:29" s="6" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="97"/>
       <c r="C87" s="7"/>
-      <c r="D87" s="286"/>
-      <c r="E87" s="286"/>
+      <c r="D87" s="287"/>
+      <c r="E87" s="287"/>
       <c r="F87" s="54"/>
-      <c r="G87" s="280"/>
-      <c r="H87" s="281"/>
-      <c r="I87" s="281"/>
-      <c r="J87" s="281"/>
-      <c r="K87" s="281"/>
-      <c r="L87" s="282"/>
+      <c r="G87" s="281"/>
+      <c r="H87" s="282"/>
+      <c r="I87" s="282"/>
+      <c r="J87" s="282"/>
+      <c r="K87" s="282"/>
+      <c r="L87" s="283"/>
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
-      <c r="P87" s="254" t="s">
+      <c r="P87" s="255" t="s">
         <v>70</v>
       </c>
-      <c r="Q87" s="255"/>
-      <c r="R87" s="255"/>
-      <c r="S87" s="255"/>
-      <c r="T87" s="255"/>
-      <c r="U87" s="255"/>
-      <c r="V87" s="255"/>
-      <c r="W87" s="255"/>
-      <c r="X87" s="256"/>
+      <c r="Q87" s="256"/>
+      <c r="R87" s="256"/>
+      <c r="S87" s="256"/>
+      <c r="T87" s="256"/>
+      <c r="U87" s="256"/>
+      <c r="V87" s="256"/>
+      <c r="W87" s="256"/>
+      <c r="X87" s="257"/>
       <c r="Y87" s="45"/>
       <c r="Z87" s="45"/>
       <c r="AA87" s="104"/>
@@ -20664,27 +20703,27 @@
     <row r="88" spans="2:29" s="6" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="97"/>
       <c r="C88" s="7"/>
-      <c r="D88" s="286"/>
-      <c r="E88" s="286"/>
+      <c r="D88" s="287"/>
+      <c r="E88" s="287"/>
       <c r="F88" s="54"/>
-      <c r="G88" s="280"/>
-      <c r="H88" s="281"/>
-      <c r="I88" s="281"/>
-      <c r="J88" s="281"/>
-      <c r="K88" s="281"/>
-      <c r="L88" s="282"/>
+      <c r="G88" s="281"/>
+      <c r="H88" s="282"/>
+      <c r="I88" s="282"/>
+      <c r="J88" s="282"/>
+      <c r="K88" s="282"/>
+      <c r="L88" s="283"/>
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
-      <c r="P88" s="257"/>
-      <c r="Q88" s="258"/>
-      <c r="R88" s="258"/>
-      <c r="S88" s="258"/>
-      <c r="T88" s="258"/>
-      <c r="U88" s="258"/>
-      <c r="V88" s="258"/>
-      <c r="W88" s="258"/>
-      <c r="X88" s="259"/>
+      <c r="P88" s="258"/>
+      <c r="Q88" s="259"/>
+      <c r="R88" s="259"/>
+      <c r="S88" s="259"/>
+      <c r="T88" s="259"/>
+      <c r="U88" s="259"/>
+      <c r="V88" s="259"/>
+      <c r="W88" s="259"/>
+      <c r="X88" s="260"/>
       <c r="Y88" s="45"/>
       <c r="Z88" s="45"/>
       <c r="AA88" s="101"/>
@@ -20694,15 +20733,15 @@
     <row r="89" spans="2:29" s="6" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="97"/>
       <c r="C89" s="7"/>
-      <c r="D89" s="286"/>
-      <c r="E89" s="286"/>
+      <c r="D89" s="287"/>
+      <c r="E89" s="287"/>
       <c r="F89" s="54"/>
-      <c r="G89" s="280"/>
-      <c r="H89" s="281"/>
-      <c r="I89" s="281"/>
-      <c r="J89" s="281"/>
-      <c r="K89" s="281"/>
-      <c r="L89" s="282"/>
+      <c r="G89" s="281"/>
+      <c r="H89" s="282"/>
+      <c r="I89" s="282"/>
+      <c r="J89" s="282"/>
+      <c r="K89" s="282"/>
+      <c r="L89" s="283"/>
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
@@ -20723,30 +20762,30 @@
     <row r="90" spans="2:29" s="6" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="97"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="286"/>
-      <c r="E90" s="286"/>
+      <c r="D90" s="287"/>
+      <c r="E90" s="287"/>
       <c r="F90" s="54"/>
-      <c r="G90" s="283"/>
-      <c r="H90" s="284"/>
-      <c r="I90" s="284"/>
-      <c r="J90" s="284"/>
-      <c r="K90" s="284"/>
-      <c r="L90" s="285"/>
+      <c r="G90" s="284"/>
+      <c r="H90" s="285"/>
+      <c r="I90" s="285"/>
+      <c r="J90" s="285"/>
+      <c r="K90" s="285"/>
+      <c r="L90" s="286"/>
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
-      <c r="P90" s="274" t="s">
+      <c r="P90" s="275" t="s">
         <v>78</v>
       </c>
-      <c r="Q90" s="275"/>
-      <c r="R90" s="276"/>
+      <c r="Q90" s="276"/>
+      <c r="R90" s="277"/>
       <c r="S90" s="45"/>
-      <c r="T90" s="274" t="s">
+      <c r="T90" s="275" t="s">
         <v>71</v>
       </c>
-      <c r="U90" s="275"/>
-      <c r="V90" s="275"/>
-      <c r="W90" s="275"/>
-      <c r="X90" s="276"/>
+      <c r="U90" s="276"/>
+      <c r="V90" s="276"/>
+      <c r="W90" s="276"/>
+      <c r="X90" s="277"/>
       <c r="Y90" s="45"/>
       <c r="Z90" s="45"/>
       <c r="AA90" s="101"/>
@@ -20767,9 +20806,9 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
-      <c r="P91" s="246"/>
-      <c r="Q91" s="246"/>
-      <c r="R91" s="246"/>
+      <c r="P91" s="247"/>
+      <c r="Q91" s="247"/>
+      <c r="R91" s="247"/>
       <c r="S91" s="49"/>
       <c r="T91" s="127"/>
       <c r="U91" s="127"/>
@@ -20789,12 +20828,12 @@
       </c>
       <c r="E92" s="49"/>
       <c r="F92" s="49"/>
-      <c r="G92" s="247"/>
-      <c r="H92" s="247"/>
-      <c r="I92" s="247"/>
-      <c r="J92" s="247"/>
-      <c r="K92" s="247"/>
-      <c r="L92" s="247"/>
+      <c r="G92" s="248"/>
+      <c r="H92" s="248"/>
+      <c r="I92" s="248"/>
+      <c r="J92" s="248"/>
+      <c r="K92" s="248"/>
+      <c r="L92" s="248"/>
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
@@ -20820,20 +20859,20 @@
       </c>
       <c r="E93" s="49"/>
       <c r="F93" s="49"/>
-      <c r="G93" s="289"/>
-      <c r="H93" s="289"/>
-      <c r="I93" s="289"/>
-      <c r="J93" s="289"/>
-      <c r="K93" s="289"/>
-      <c r="L93" s="289"/>
+      <c r="G93" s="290"/>
+      <c r="H93" s="290"/>
+      <c r="I93" s="290"/>
+      <c r="J93" s="290"/>
+      <c r="K93" s="290"/>
+      <c r="L93" s="290"/>
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
-      <c r="P93" s="287" t="s">
+      <c r="P93" s="288" t="s">
         <v>79</v>
       </c>
-      <c r="Q93" s="287"/>
-      <c r="R93" s="287"/>
+      <c r="Q93" s="288"/>
+      <c r="R93" s="288"/>
       <c r="S93" s="27"/>
       <c r="T93" s="27"/>
       <c r="U93" s="27"/>
@@ -20853,18 +20892,18 @@
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
-      <c r="G94" s="288"/>
-      <c r="H94" s="288"/>
-      <c r="I94" s="288"/>
-      <c r="J94" s="288"/>
-      <c r="K94" s="288"/>
-      <c r="L94" s="288"/>
+      <c r="G94" s="289"/>
+      <c r="H94" s="289"/>
+      <c r="I94" s="289"/>
+      <c r="J94" s="289"/>
+      <c r="K94" s="289"/>
+      <c r="L94" s="289"/>
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
-      <c r="P94" s="287"/>
-      <c r="Q94" s="287"/>
-      <c r="R94" s="287"/>
+      <c r="P94" s="288"/>
+      <c r="Q94" s="288"/>
+      <c r="R94" s="288"/>
       <c r="S94" s="27"/>
       <c r="T94" s="27"/>
       <c r="U94" s="27"/>
@@ -20879,10 +20918,10 @@
     <row r="95" spans="2:29" s="6" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B95" s="97"/>
       <c r="C95" s="7"/>
-      <c r="D95" s="245" t="s">
+      <c r="D95" s="246" t="s">
         <v>102</v>
       </c>
-      <c r="E95" s="245"/>
+      <c r="E95" s="246"/>
       <c r="F95" s="48"/>
       <c r="G95" s="203"/>
       <c r="H95" s="203"/>
@@ -20895,9 +20934,9 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
-      <c r="P95" s="290"/>
-      <c r="Q95" s="290"/>
-      <c r="R95" s="290"/>
+      <c r="P95" s="291"/>
+      <c r="Q95" s="291"/>
+      <c r="R95" s="291"/>
       <c r="S95" s="27"/>
       <c r="T95" s="27"/>
       <c r="U95" s="27"/>
@@ -20923,19 +20962,19 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
-      <c r="P96" s="248" t="s">
+      <c r="P96" s="249" t="s">
         <v>107</v>
       </c>
-      <c r="Q96" s="249"/>
-      <c r="R96" s="250"/>
-      <c r="S96" s="272"/>
-      <c r="T96" s="248" t="s">
+      <c r="Q96" s="250"/>
+      <c r="R96" s="251"/>
+      <c r="S96" s="273"/>
+      <c r="T96" s="249" t="s">
         <v>107</v>
       </c>
-      <c r="U96" s="249"/>
-      <c r="V96" s="249"/>
-      <c r="W96" s="249"/>
-      <c r="X96" s="250"/>
+      <c r="U96" s="250"/>
+      <c r="V96" s="250"/>
+      <c r="W96" s="250"/>
+      <c r="X96" s="251"/>
       <c r="Y96" s="40"/>
       <c r="Z96" s="40"/>
       <c r="AA96" s="104"/>
@@ -20963,14 +21002,14 @@
       </c>
       <c r="Q97" s="43"/>
       <c r="R97" s="131"/>
-      <c r="S97" s="273"/>
-      <c r="T97" s="266" t="s">
+      <c r="S97" s="274"/>
+      <c r="T97" s="267" t="s">
         <v>35</v>
       </c>
-      <c r="U97" s="267"/>
-      <c r="V97" s="267"/>
-      <c r="W97" s="267"/>
-      <c r="X97" s="268"/>
+      <c r="U97" s="268"/>
+      <c r="V97" s="268"/>
+      <c r="W97" s="268"/>
+      <c r="X97" s="269"/>
       <c r="Y97" s="7"/>
       <c r="Z97" s="7"/>
       <c r="AA97" s="104"/>
@@ -20996,14 +21035,14 @@
       </c>
       <c r="Q98" s="43"/>
       <c r="R98" s="43"/>
-      <c r="S98" s="273"/>
-      <c r="T98" s="269" t="s">
+      <c r="S98" s="274"/>
+      <c r="T98" s="270" t="s">
         <v>36</v>
       </c>
-      <c r="U98" s="270"/>
-      <c r="V98" s="270"/>
-      <c r="W98" s="270"/>
-      <c r="X98" s="271"/>
+      <c r="U98" s="271"/>
+      <c r="V98" s="271"/>
+      <c r="W98" s="271"/>
+      <c r="X98" s="272"/>
       <c r="Y98" s="7"/>
       <c r="Z98" s="7"/>
       <c r="AA98" s="104"/>
@@ -21188,8 +21227,8 @@
     <hyperlink ref="R37" r:id="rId2" xr:uid="{985289E6-07C6-4D3B-B395-DFD0D771F3AC}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.51181102362204722" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="53" orientation="portrait" r:id="rId3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="52" orientation="portrait" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddHeader xml:space="preserve">&amp;C                                                        </oddHeader>
     <oddFooter>&amp;LVersión 01                Fecha:                   7/7/2017&amp;CPágina 1 de 1&amp;RCódigo RE-M-IN-74</oddFooter>
@@ -21659,8 +21698,8 @@
       <c r="Y5" s="214"/>
       <c r="Z5" s="215"/>
       <c r="AA5" s="99"/>
-      <c r="AB5" s="295" t="s">
-        <v>165</v>
+      <c r="AB5" s="296" t="s">
+        <v>164</v>
       </c>
       <c r="AC5" s="30"/>
     </row>
@@ -21692,7 +21731,7 @@
       <c r="Y6" s="201"/>
       <c r="Z6" s="201"/>
       <c r="AA6" s="100"/>
-      <c r="AB6" s="295"/>
+      <c r="AB6" s="296"/>
       <c r="AC6" s="30"/>
     </row>
     <row r="7" spans="1:29" s="8" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -21743,7 +21782,7 @@
         <v>31</v>
       </c>
       <c r="AA7" s="100"/>
-      <c r="AB7" s="295"/>
+      <c r="AB7" s="296"/>
       <c r="AC7" s="2"/>
     </row>
     <row r="8" spans="1:29" s="6" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -21779,7 +21818,7 @@
         <v>2023</v>
       </c>
       <c r="AA8" s="101"/>
-      <c r="AB8" s="295"/>
+      <c r="AB8" s="296"/>
       <c r="AC8" s="2"/>
     </row>
     <row r="9" spans="1:29" s="6" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -21840,8 +21879,8 @@
       <c r="Y10" s="180"/>
       <c r="Z10" s="180"/>
       <c r="AA10" s="101"/>
-      <c r="AB10" s="293" t="s">
-        <v>166</v>
+      <c r="AB10" s="294" t="s">
+        <v>165</v>
       </c>
       <c r="AC10" s="2"/>
     </row>
@@ -21872,7 +21911,7 @@
       <c r="Y11" s="202"/>
       <c r="Z11" s="202"/>
       <c r="AA11" s="101"/>
-      <c r="AB11" s="294"/>
+      <c r="AB11" s="295"/>
       <c r="AC11" s="2"/>
     </row>
     <row r="12" spans="1:29" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21908,7 +21947,7 @@
         <v>31</v>
       </c>
       <c r="AA12" s="98"/>
-      <c r="AB12" s="294"/>
+      <c r="AB12" s="295"/>
       <c r="AC12" s="3"/>
     </row>
     <row r="13" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -21956,7 +21995,7 @@
         <v>2023</v>
       </c>
       <c r="AA13" s="100"/>
-      <c r="AB13" s="294"/>
+      <c r="AB13" s="295"/>
       <c r="AC13" s="2"/>
     </row>
     <row r="14" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -21986,7 +22025,7 @@
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
       <c r="AA14" s="100"/>
-      <c r="AB14" s="294"/>
+      <c r="AB14" s="295"/>
       <c r="AC14" s="34"/>
     </row>
     <row r="15" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -22000,16 +22039,16 @@
         <v>91</v>
       </c>
       <c r="H15" s="29"/>
-      <c r="I15" s="236">
+      <c r="I15" s="237">
         <v>44991</v>
       </c>
-      <c r="J15" s="237"/>
-      <c r="K15" s="237"/>
-      <c r="L15" s="237"/>
-      <c r="M15" s="237"/>
-      <c r="N15" s="237"/>
-      <c r="O15" s="237"/>
-      <c r="P15" s="238"/>
+      <c r="J15" s="238"/>
+      <c r="K15" s="238"/>
+      <c r="L15" s="238"/>
+      <c r="M15" s="238"/>
+      <c r="N15" s="238"/>
+      <c r="O15" s="238"/>
+      <c r="P15" s="239"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="172" t="s">
         <v>4</v>
@@ -22029,7 +22068,7 @@
         <v>2023</v>
       </c>
       <c r="AA15" s="100"/>
-      <c r="AB15" s="294"/>
+      <c r="AB15" s="295"/>
       <c r="AC15" s="2"/>
     </row>
     <row r="16" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22044,20 +22083,20 @@
         <v>51</v>
       </c>
       <c r="H16" s="49"/>
-      <c r="I16" s="234">
+      <c r="I16" s="235">
         <v>2323</v>
       </c>
-      <c r="J16" s="234"/>
+      <c r="J16" s="235"/>
       <c r="K16" s="45" t="s">
         <v>5</v>
       </c>
       <c r="L16" s="49"/>
-      <c r="M16" s="235">
+      <c r="M16" s="236">
         <v>44985</v>
       </c>
-      <c r="N16" s="235"/>
-      <c r="O16" s="235"/>
-      <c r="P16" s="235"/>
+      <c r="N16" s="236"/>
+      <c r="O16" s="236"/>
+      <c r="P16" s="236"/>
       <c r="Q16" s="45"/>
       <c r="R16" s="7" t="s">
         <v>6</v>
@@ -22079,7 +22118,7 @@
         <v>103</v>
       </c>
       <c r="AA16" s="104"/>
-      <c r="AB16" s="294"/>
+      <c r="AB16" s="295"/>
       <c r="AC16" s="2"/>
     </row>
     <row r="17" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -22100,19 +22139,19 @@
         <v>8</v>
       </c>
       <c r="L17" s="49"/>
-      <c r="M17" s="239">
+      <c r="M17" s="240">
         <v>44991</v>
       </c>
-      <c r="N17" s="239"/>
-      <c r="O17" s="239"/>
-      <c r="P17" s="239"/>
+      <c r="N17" s="240"/>
+      <c r="O17" s="240"/>
+      <c r="P17" s="240"/>
       <c r="Q17" s="45"/>
       <c r="R17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="S17" s="7"/>
       <c r="T17" s="198" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U17" s="198"/>
       <c r="V17" s="198"/>
@@ -22121,7 +22160,7 @@
       <c r="Y17" s="198"/>
       <c r="Z17" s="198"/>
       <c r="AA17" s="100"/>
-      <c r="AB17" s="294"/>
+      <c r="AB17" s="295"/>
       <c r="AC17" s="2"/>
     </row>
     <row r="18" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22153,7 +22192,7 @@
       <c r="Y18" s="194"/>
       <c r="Z18" s="194"/>
       <c r="AA18" s="100"/>
-      <c r="AB18" s="294"/>
+      <c r="AB18" s="295"/>
       <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22172,10 +22211,10 @@
         <v>8</v>
       </c>
       <c r="L19" s="49"/>
-      <c r="M19" s="240"/>
-      <c r="N19" s="240"/>
-      <c r="O19" s="240"/>
-      <c r="P19" s="240"/>
+      <c r="M19" s="241"/>
+      <c r="N19" s="241"/>
+      <c r="O19" s="241"/>
+      <c r="P19" s="241"/>
       <c r="Q19" s="49"/>
       <c r="R19" s="49"/>
       <c r="S19" s="49"/>
@@ -22187,7 +22226,7 @@
       <c r="Y19" s="194"/>
       <c r="Z19" s="194"/>
       <c r="AA19" s="100"/>
-      <c r="AB19" s="294"/>
+      <c r="AB19" s="295"/>
       <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29" s="6" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -22217,7 +22256,7 @@
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
       <c r="AA20" s="100"/>
-      <c r="AB20" s="294"/>
+      <c r="AB20" s="295"/>
       <c r="AC20" s="2"/>
     </row>
     <row r="21" spans="1:29" s="6" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -22247,7 +22286,7 @@
       <c r="Y21" s="121"/>
       <c r="Z21" s="123"/>
       <c r="AA21" s="100"/>
-      <c r="AB21" s="294"/>
+      <c r="AB21" s="295"/>
       <c r="AC21" s="2"/>
     </row>
     <row r="22" spans="1:29" s="6" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -22259,7 +22298,7 @@
       <c r="E22" s="166"/>
       <c r="F22" s="167"/>
       <c r="G22" s="204" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H22" s="205"/>
       <c r="I22" s="205"/>
@@ -22281,7 +22320,7 @@
       <c r="Y22" s="205"/>
       <c r="Z22" s="206"/>
       <c r="AA22" s="99"/>
-      <c r="AB22" s="294"/>
+      <c r="AB22" s="295"/>
       <c r="AC22" s="2"/>
     </row>
     <row r="23" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -22343,8 +22382,8 @@
       <c r="Y24" s="164"/>
       <c r="Z24" s="165"/>
       <c r="AA24" s="98"/>
-      <c r="AB24" s="293" t="s">
-        <v>164</v>
+      <c r="AB24" s="294" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:29" s="7" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -22361,7 +22400,7 @@
       <c r="L25" s="90"/>
       <c r="M25" s="90"/>
       <c r="AA25" s="104"/>
-      <c r="AB25" s="294"/>
+      <c r="AB25" s="295"/>
     </row>
     <row r="26" spans="1:29" s="33" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="84"/>
@@ -22389,7 +22428,7 @@
         <v>87</v>
       </c>
       <c r="AA26" s="110"/>
-      <c r="AB26" s="294"/>
+      <c r="AB26" s="295"/>
     </row>
     <row r="27" spans="1:29" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="84"/>
@@ -22420,7 +22459,7 @@
       <c r="Y27" s="80"/>
       <c r="Z27" s="80"/>
       <c r="AA27" s="111"/>
-      <c r="AB27" s="294"/>
+      <c r="AB27" s="295"/>
     </row>
     <row r="28" spans="1:29" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="84"/>
@@ -22451,7 +22490,7 @@
       <c r="Y28" s="80"/>
       <c r="Z28" s="80"/>
       <c r="AA28" s="111"/>
-      <c r="AB28" s="294"/>
+      <c r="AB28" s="295"/>
     </row>
     <row r="29" spans="1:29" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="84"/>
@@ -22463,7 +22502,7 @@
       <c r="F29" s="186"/>
       <c r="G29" s="186"/>
       <c r="H29" s="160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I29" s="160"/>
       <c r="J29" s="160"/>
@@ -22484,7 +22523,7 @@
       <c r="Y29" s="80"/>
       <c r="Z29" s="80"/>
       <c r="AA29" s="111"/>
-      <c r="AB29" s="294"/>
+      <c r="AB29" s="295"/>
     </row>
     <row r="30" spans="1:29" s="84" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="109"/>
@@ -22496,7 +22535,7 @@
       <c r="F30" s="186"/>
       <c r="G30" s="186"/>
       <c r="H30" s="160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I30" s="160"/>
       <c r="J30" s="160"/>
@@ -22517,7 +22556,7 @@
       <c r="Y30" s="80"/>
       <c r="Z30" s="80"/>
       <c r="AA30" s="111"/>
-      <c r="AB30" s="294"/>
+      <c r="AB30" s="295"/>
       <c r="AC30" s="1"/>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -22540,7 +22579,7 @@
       <c r="R31" s="48"/>
       <c r="S31" s="48"/>
       <c r="AA31" s="104"/>
-      <c r="AB31" s="294"/>
+      <c r="AB31" s="295"/>
       <c r="AC31" s="2"/>
     </row>
     <row r="32" spans="1:29" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -22572,8 +22611,8 @@
       <c r="Y32" s="228"/>
       <c r="Z32" s="229"/>
       <c r="AA32" s="101"/>
-      <c r="AB32" s="293" t="s">
-        <v>167</v>
+      <c r="AB32" s="294" t="s">
+        <v>166</v>
       </c>
       <c r="AC32" s="2"/>
     </row>
@@ -22604,7 +22643,7 @@
       <c r="Y33" s="171"/>
       <c r="Z33" s="171"/>
       <c r="AA33" s="101"/>
-      <c r="AB33" s="293"/>
+      <c r="AB33" s="294"/>
       <c r="AC33" s="2"/>
     </row>
     <row r="34" spans="1:29" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -22616,7 +22655,7 @@
       <c r="E34" s="172"/>
       <c r="F34" s="49"/>
       <c r="G34" s="173" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H34" s="174"/>
       <c r="I34" s="174"/>
@@ -22638,7 +22677,7 @@
       <c r="Y34" s="174"/>
       <c r="Z34" s="175"/>
       <c r="AA34" s="105"/>
-      <c r="AB34" s="293"/>
+      <c r="AB34" s="294"/>
       <c r="AC34" s="2"/>
     </row>
     <row r="35" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -22668,7 +22707,7 @@
       <c r="Y35" s="49"/>
       <c r="Z35" s="49"/>
       <c r="AA35" s="105"/>
-      <c r="AB35" s="293"/>
+      <c r="AB35" s="294"/>
       <c r="AC35" s="2"/>
     </row>
     <row r="36" spans="1:29" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -22696,16 +22735,16 @@
         <v>3</v>
       </c>
       <c r="Q36" s="45"/>
-      <c r="R36" s="231">
+      <c r="R36" s="232">
         <v>123456789</v>
       </c>
-      <c r="S36" s="232"/>
-      <c r="T36" s="233"/>
+      <c r="S36" s="233"/>
+      <c r="T36" s="234"/>
       <c r="X36" s="45"/>
       <c r="Y36" s="45"/>
       <c r="Z36" s="85"/>
       <c r="AA36" s="104"/>
-      <c r="AB36" s="293"/>
+      <c r="AB36" s="294"/>
       <c r="AC36" s="2"/>
     </row>
     <row r="37" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22717,22 +22756,22 @@
       <c r="E37" s="172"/>
       <c r="F37" s="49"/>
       <c r="G37" s="185" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H37" s="185"/>
       <c r="I37" s="185"/>
       <c r="J37" s="185"/>
       <c r="K37" s="185"/>
       <c r="L37" s="18"/>
-      <c r="M37" s="230" t="s">
+      <c r="M37" s="231" t="s">
         <v>98</v>
       </c>
-      <c r="N37" s="230"/>
-      <c r="O37" s="230"/>
-      <c r="P37" s="230"/>
+      <c r="N37" s="231"/>
+      <c r="O37" s="231"/>
+      <c r="P37" s="231"/>
       <c r="Q37" s="18"/>
-      <c r="R37" s="296" t="s">
-        <v>162</v>
+      <c r="R37" s="230" t="s">
+        <v>161</v>
       </c>
       <c r="S37" s="185"/>
       <c r="T37" s="185"/>
@@ -22743,7 +22782,7 @@
       <c r="Y37" s="185"/>
       <c r="Z37" s="185"/>
       <c r="AA37" s="106"/>
-      <c r="AB37" s="293"/>
+      <c r="AB37" s="294"/>
       <c r="AC37" s="2"/>
     </row>
     <row r="38" spans="1:29" s="7" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22773,7 +22812,7 @@
       <c r="Y38" s="18"/>
       <c r="Z38" s="18"/>
       <c r="AA38" s="107"/>
-      <c r="AB38" s="293"/>
+      <c r="AB38" s="294"/>
       <c r="AC38" s="2"/>
     </row>
     <row r="39" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22784,13 +22823,13 @@
       </c>
       <c r="E39" s="172"/>
       <c r="F39" s="49"/>
-      <c r="G39" s="243">
+      <c r="G39" s="244">
         <v>3058974526</v>
       </c>
-      <c r="H39" s="243"/>
-      <c r="I39" s="243"/>
-      <c r="J39" s="243"/>
-      <c r="K39" s="243"/>
+      <c r="H39" s="244"/>
+      <c r="I39" s="244"/>
+      <c r="J39" s="244"/>
+      <c r="K39" s="244"/>
       <c r="M39" s="7" t="s">
         <v>37</v>
       </c>
@@ -22810,7 +22849,7 @@
       <c r="Y39" s="203"/>
       <c r="Z39" s="203"/>
       <c r="AA39" s="104"/>
-      <c r="AB39" s="293"/>
+      <c r="AB39" s="294"/>
       <c r="AC39" s="2"/>
     </row>
     <row r="40" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -22838,7 +22877,7 @@
       <c r="Y40" s="45"/>
       <c r="Z40" s="45"/>
       <c r="AA40" s="100"/>
-      <c r="AB40" s="293"/>
+      <c r="AB40" s="294"/>
       <c r="AC40" s="2"/>
     </row>
     <row r="41" spans="1:29" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22858,7 +22897,7 @@
         <v>3</v>
       </c>
       <c r="N41" s="183" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O41" s="183"/>
       <c r="P41" s="183"/>
@@ -22877,7 +22916,7 @@
       <c r="Y41" s="184"/>
       <c r="Z41" s="184"/>
       <c r="AA41" s="100"/>
-      <c r="AB41" s="293"/>
+      <c r="AB41" s="294"/>
       <c r="AC41" s="2"/>
     </row>
     <row r="42" spans="1:29" s="7" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22905,7 +22944,7 @@
       <c r="Y42" s="45"/>
       <c r="Z42" s="45"/>
       <c r="AA42" s="100"/>
-      <c r="AB42" s="293"/>
+      <c r="AB42" s="294"/>
       <c r="AC42" s="2"/>
     </row>
     <row r="43" spans="1:29" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22935,7 +22974,7 @@
       <c r="Y43" s="45"/>
       <c r="Z43" s="45"/>
       <c r="AA43" s="101"/>
-      <c r="AB43" s="293"/>
+      <c r="AB43" s="294"/>
     </row>
     <row r="44" spans="1:29" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="97"/>
@@ -23084,9 +23123,9 @@
         <v>3</v>
       </c>
       <c r="Q48" s="45"/>
-      <c r="R48" s="231"/>
-      <c r="S48" s="232"/>
-      <c r="T48" s="233"/>
+      <c r="R48" s="232"/>
+      <c r="S48" s="233"/>
+      <c r="T48" s="234"/>
       <c r="X48" s="45"/>
       <c r="Y48" s="45"/>
       <c r="Z48" s="85"/>
@@ -23108,12 +23147,12 @@
       <c r="J49" s="185"/>
       <c r="K49" s="185"/>
       <c r="L49" s="18"/>
-      <c r="M49" s="230" t="s">
+      <c r="M49" s="231" t="s">
         <v>98</v>
       </c>
-      <c r="N49" s="230"/>
-      <c r="O49" s="230"/>
-      <c r="P49" s="230"/>
+      <c r="N49" s="231"/>
+      <c r="O49" s="231"/>
+      <c r="P49" s="231"/>
       <c r="Q49" s="18"/>
       <c r="R49" s="185"/>
       <c r="S49" s="185"/>
@@ -23166,11 +23205,11 @@
       </c>
       <c r="E51" s="172"/>
       <c r="F51" s="49"/>
-      <c r="G51" s="243"/>
-      <c r="H51" s="243"/>
-      <c r="I51" s="243"/>
-      <c r="J51" s="243"/>
-      <c r="K51" s="243"/>
+      <c r="G51" s="244"/>
+      <c r="H51" s="244"/>
+      <c r="I51" s="244"/>
+      <c r="J51" s="244"/>
+      <c r="K51" s="244"/>
       <c r="M51" s="7" t="s">
         <v>37</v>
       </c>
@@ -23338,8 +23377,8 @@
       <c r="Y56" s="180"/>
       <c r="Z56" s="180"/>
       <c r="AA56" s="101"/>
-      <c r="AB56" s="295" t="s">
-        <v>168</v>
+      <c r="AB56" s="296" t="s">
+        <v>167</v>
       </c>
       <c r="AC56" s="2"/>
     </row>
@@ -23370,7 +23409,7 @@
       <c r="Y57" s="51"/>
       <c r="Z57" s="51"/>
       <c r="AA57" s="101"/>
-      <c r="AB57" s="295"/>
+      <c r="AB57" s="296"/>
       <c r="AC57" s="2"/>
     </row>
     <row r="58" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23401,7 +23440,7 @@
       <c r="Y58" s="22"/>
       <c r="Z58" s="22"/>
       <c r="AA58" s="104"/>
-      <c r="AB58" s="295"/>
+      <c r="AB58" s="296"/>
       <c r="AC58" s="2"/>
     </row>
     <row r="59" spans="1:29" s="7" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
@@ -23429,7 +23468,7 @@
       <c r="Y59" s="22"/>
       <c r="Z59" s="22"/>
       <c r="AA59" s="104"/>
-      <c r="AB59" s="295"/>
+      <c r="AB59" s="296"/>
       <c r="AC59" s="2"/>
     </row>
     <row r="60" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23460,7 +23499,7 @@
       <c r="Y60" s="22"/>
       <c r="Z60" s="22"/>
       <c r="AA60" s="104"/>
-      <c r="AB60" s="295"/>
+      <c r="AB60" s="296"/>
       <c r="AC60" s="2"/>
     </row>
     <row r="61" spans="1:29" s="7" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23485,7 +23524,7 @@
       <c r="Y61" s="22"/>
       <c r="Z61" s="22"/>
       <c r="AA61" s="104"/>
-      <c r="AB61" s="295"/>
+      <c r="AB61" s="296"/>
       <c r="AC61" s="2"/>
     </row>
     <row r="62" spans="1:29" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23519,7 +23558,7 @@
       <c r="Y62" s="22"/>
       <c r="Z62" s="22"/>
       <c r="AA62" s="104"/>
-      <c r="AB62" s="295"/>
+      <c r="AB62" s="296"/>
       <c r="AC62" s="2"/>
     </row>
     <row r="63" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -23544,7 +23583,7 @@
       <c r="Y63" s="22"/>
       <c r="Z63" s="22"/>
       <c r="AA63" s="104"/>
-      <c r="AB63" s="295"/>
+      <c r="AB63" s="296"/>
       <c r="AC63" s="2"/>
     </row>
     <row r="64" spans="1:29" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23579,7 +23618,7 @@
       <c r="Y64" s="25"/>
       <c r="Z64" s="25"/>
       <c r="AA64" s="108"/>
-      <c r="AB64" s="295"/>
+      <c r="AB64" s="296"/>
       <c r="AC64" s="2"/>
     </row>
     <row r="65" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23612,7 +23651,7 @@
       <c r="Y65" s="25"/>
       <c r="Z65" s="25"/>
       <c r="AA65" s="108"/>
-      <c r="AB65" s="295"/>
+      <c r="AB65" s="296"/>
       <c r="AC65" s="2"/>
     </row>
     <row r="66" spans="1:29" s="7" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23639,7 +23678,7 @@
       <c r="Y66" s="25"/>
       <c r="Z66" s="25"/>
       <c r="AA66" s="108"/>
-      <c r="AB66" s="295"/>
+      <c r="AB66" s="296"/>
       <c r="AC66" s="2"/>
     </row>
     <row r="67" spans="1:29" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23674,7 +23713,7 @@
       <c r="Y67" s="25"/>
       <c r="Z67" s="25"/>
       <c r="AA67" s="108"/>
-      <c r="AB67" s="295"/>
+      <c r="AB67" s="296"/>
       <c r="AC67" s="2"/>
     </row>
     <row r="68" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23703,7 +23742,7 @@
       <c r="Y68" s="25"/>
       <c r="Z68" s="25"/>
       <c r="AA68" s="108"/>
-      <c r="AB68" s="295"/>
+      <c r="AB68" s="296"/>
       <c r="AC68" s="2"/>
     </row>
     <row r="69" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -23730,7 +23769,7 @@
       <c r="Y69" s="25"/>
       <c r="Z69" s="25"/>
       <c r="AA69" s="108"/>
-      <c r="AB69" s="295"/>
+      <c r="AB69" s="296"/>
       <c r="AC69" s="2"/>
     </row>
     <row r="70" spans="1:29" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23765,7 +23804,7 @@
       <c r="Y70" s="25"/>
       <c r="Z70" s="25"/>
       <c r="AA70" s="108"/>
-      <c r="AB70" s="295"/>
+      <c r="AB70" s="296"/>
       <c r="AC70" s="2"/>
     </row>
     <row r="71" spans="1:29" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23800,7 +23839,7 @@
       <c r="Y71" s="25"/>
       <c r="Z71" s="25"/>
       <c r="AA71" s="112"/>
-      <c r="AB71" s="295"/>
+      <c r="AB71" s="296"/>
       <c r="AC71" s="2"/>
     </row>
     <row r="72" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -23825,7 +23864,7 @@
       <c r="Y72" s="22"/>
       <c r="Z72" s="22"/>
       <c r="AA72" s="112"/>
-      <c r="AB72" s="295"/>
+      <c r="AB72" s="296"/>
       <c r="AC72" s="2"/>
     </row>
     <row r="73" spans="1:29" s="7" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -23850,7 +23889,7 @@
       <c r="Y73" s="22"/>
       <c r="Z73" s="22"/>
       <c r="AA73" s="112"/>
-      <c r="AB73" s="295"/>
+      <c r="AB73" s="296"/>
       <c r="AC73" s="2"/>
     </row>
     <row r="74" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23885,7 +23924,7 @@
       <c r="Y74" s="7"/>
       <c r="Z74" s="79"/>
       <c r="AA74" s="113"/>
-      <c r="AB74" s="295"/>
+      <c r="AB74" s="296"/>
       <c r="AC74" s="2"/>
     </row>
     <row r="75" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23919,7 +23958,7 @@
       <c r="Y75" s="7"/>
       <c r="Z75" s="48"/>
       <c r="AA75" s="99"/>
-      <c r="AB75" s="295"/>
+      <c r="AB75" s="296"/>
       <c r="AC75" s="2"/>
     </row>
     <row r="76" spans="1:29" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23954,7 +23993,7 @@
       <c r="Y76" s="7"/>
       <c r="Z76" s="48"/>
       <c r="AA76" s="114"/>
-      <c r="AB76" s="295"/>
+      <c r="AB76" s="296"/>
       <c r="AC76" s="2"/>
     </row>
     <row r="77" spans="1:29" s="6" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23984,37 +24023,37 @@
       <c r="Y77" s="7"/>
       <c r="Z77" s="7"/>
       <c r="AA77" s="114"/>
-      <c r="AB77" s="295"/>
+      <c r="AB77" s="296"/>
       <c r="AC77" s="2"/>
     </row>
     <row r="78" spans="1:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="97"/>
-      <c r="C78" s="260" t="s">
+      <c r="C78" s="261" t="s">
         <v>100</v>
       </c>
-      <c r="D78" s="261"/>
-      <c r="E78" s="261"/>
-      <c r="F78" s="244"/>
-      <c r="G78" s="244"/>
-      <c r="H78" s="244"/>
-      <c r="I78" s="244"/>
-      <c r="J78" s="244"/>
-      <c r="K78" s="244"/>
-      <c r="L78" s="244"/>
-      <c r="M78" s="244"/>
-      <c r="N78" s="244"/>
-      <c r="O78" s="244"/>
-      <c r="P78" s="252" t="s">
+      <c r="D78" s="262"/>
+      <c r="E78" s="262"/>
+      <c r="F78" s="245"/>
+      <c r="G78" s="245"/>
+      <c r="H78" s="245"/>
+      <c r="I78" s="245"/>
+      <c r="J78" s="245"/>
+      <c r="K78" s="245"/>
+      <c r="L78" s="245"/>
+      <c r="M78" s="245"/>
+      <c r="N78" s="245"/>
+      <c r="O78" s="245"/>
+      <c r="P78" s="253" t="s">
         <v>83</v>
       </c>
-      <c r="Q78" s="253"/>
-      <c r="R78" s="253"/>
-      <c r="S78" s="253"/>
-      <c r="T78" s="253"/>
-      <c r="U78" s="253"/>
-      <c r="V78" s="253"/>
-      <c r="W78" s="253"/>
-      <c r="X78" s="253"/>
+      <c r="Q78" s="254"/>
+      <c r="R78" s="254"/>
+      <c r="S78" s="254"/>
+      <c r="T78" s="254"/>
+      <c r="U78" s="254"/>
+      <c r="V78" s="254"/>
+      <c r="W78" s="254"/>
+      <c r="X78" s="254"/>
       <c r="Y78" s="7"/>
       <c r="Z78" s="7"/>
       <c r="AA78" s="114"/>
@@ -24023,25 +24062,25 @@
     </row>
     <row r="79" spans="1:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="97"/>
-      <c r="C79" s="262"/>
-      <c r="D79" s="263"/>
-      <c r="E79" s="263"/>
-      <c r="F79" s="244"/>
-      <c r="G79" s="244"/>
-      <c r="H79" s="244"/>
-      <c r="I79" s="244"/>
-      <c r="J79" s="244"/>
-      <c r="K79" s="244"/>
-      <c r="L79" s="244"/>
-      <c r="M79" s="244"/>
-      <c r="N79" s="244"/>
-      <c r="O79" s="244"/>
-      <c r="P79" s="251" t="s">
+      <c r="C79" s="263"/>
+      <c r="D79" s="264"/>
+      <c r="E79" s="264"/>
+      <c r="F79" s="245"/>
+      <c r="G79" s="245"/>
+      <c r="H79" s="245"/>
+      <c r="I79" s="245"/>
+      <c r="J79" s="245"/>
+      <c r="K79" s="245"/>
+      <c r="L79" s="245"/>
+      <c r="M79" s="245"/>
+      <c r="N79" s="245"/>
+      <c r="O79" s="245"/>
+      <c r="P79" s="252" t="s">
         <v>35</v>
       </c>
       <c r="Q79" s="200"/>
       <c r="R79" s="200" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S79" s="200"/>
       <c r="T79" s="200"/>
@@ -24057,20 +24096,20 @@
     </row>
     <row r="80" spans="1:29" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="97"/>
-      <c r="C80" s="264"/>
-      <c r="D80" s="265"/>
-      <c r="E80" s="265"/>
-      <c r="F80" s="244"/>
-      <c r="G80" s="244"/>
-      <c r="H80" s="244"/>
-      <c r="I80" s="244"/>
-      <c r="J80" s="244"/>
-      <c r="K80" s="244"/>
-      <c r="L80" s="244"/>
-      <c r="M80" s="244"/>
-      <c r="N80" s="244"/>
-      <c r="O80" s="244"/>
-      <c r="P80" s="251" t="s">
+      <c r="C80" s="265"/>
+      <c r="D80" s="266"/>
+      <c r="E80" s="266"/>
+      <c r="F80" s="245"/>
+      <c r="G80" s="245"/>
+      <c r="H80" s="245"/>
+      <c r="I80" s="245"/>
+      <c r="J80" s="245"/>
+      <c r="K80" s="245"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="245"/>
+      <c r="N80" s="245"/>
+      <c r="O80" s="245"/>
+      <c r="P80" s="252" t="s">
         <v>33</v>
       </c>
       <c r="Q80" s="200"/>
@@ -24089,62 +24128,62 @@
     </row>
     <row r="81" spans="2:29" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="97"/>
-      <c r="C81" s="241"/>
-      <c r="D81" s="242"/>
-      <c r="E81" s="242"/>
-      <c r="F81" s="242"/>
-      <c r="G81" s="242"/>
-      <c r="H81" s="242"/>
-      <c r="I81" s="242"/>
-      <c r="J81" s="242"/>
-      <c r="K81" s="242"/>
-      <c r="L81" s="242"/>
-      <c r="M81" s="242"/>
-      <c r="N81" s="242"/>
-      <c r="O81" s="242"/>
-      <c r="P81" s="242"/>
-      <c r="Q81" s="242"/>
-      <c r="R81" s="242"/>
-      <c r="S81" s="242"/>
-      <c r="T81" s="242"/>
-      <c r="U81" s="242"/>
-      <c r="V81" s="242"/>
-      <c r="W81" s="242"/>
-      <c r="X81" s="242"/>
-      <c r="Y81" s="242"/>
-      <c r="Z81" s="242"/>
+      <c r="C81" s="242"/>
+      <c r="D81" s="243"/>
+      <c r="E81" s="243"/>
+      <c r="F81" s="243"/>
+      <c r="G81" s="243"/>
+      <c r="H81" s="243"/>
+      <c r="I81" s="243"/>
+      <c r="J81" s="243"/>
+      <c r="K81" s="243"/>
+      <c r="L81" s="243"/>
+      <c r="M81" s="243"/>
+      <c r="N81" s="243"/>
+      <c r="O81" s="243"/>
+      <c r="P81" s="243"/>
+      <c r="Q81" s="243"/>
+      <c r="R81" s="243"/>
+      <c r="S81" s="243"/>
+      <c r="T81" s="243"/>
+      <c r="U81" s="243"/>
+      <c r="V81" s="243"/>
+      <c r="W81" s="243"/>
+      <c r="X81" s="243"/>
+      <c r="Y81" s="243"/>
+      <c r="Z81" s="243"/>
       <c r="AA81" s="99"/>
       <c r="AB81" s="134"/>
       <c r="AC81" s="2"/>
     </row>
     <row r="82" spans="2:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="97"/>
-      <c r="C82" s="260" t="s">
+      <c r="C82" s="261" t="s">
         <v>105</v>
       </c>
-      <c r="D82" s="261"/>
-      <c r="E82" s="261"/>
-      <c r="F82" s="291"/>
-      <c r="G82" s="292"/>
-      <c r="H82" s="292"/>
-      <c r="I82" s="292"/>
-      <c r="J82" s="292"/>
-      <c r="K82" s="292"/>
-      <c r="L82" s="292"/>
-      <c r="M82" s="292"/>
-      <c r="N82" s="292"/>
-      <c r="O82" s="292"/>
-      <c r="P82" s="252" t="s">
+      <c r="D82" s="262"/>
+      <c r="E82" s="262"/>
+      <c r="F82" s="292"/>
+      <c r="G82" s="293"/>
+      <c r="H82" s="293"/>
+      <c r="I82" s="293"/>
+      <c r="J82" s="293"/>
+      <c r="K82" s="293"/>
+      <c r="L82" s="293"/>
+      <c r="M82" s="293"/>
+      <c r="N82" s="293"/>
+      <c r="O82" s="293"/>
+      <c r="P82" s="253" t="s">
         <v>106</v>
       </c>
-      <c r="Q82" s="253"/>
-      <c r="R82" s="253"/>
-      <c r="S82" s="253"/>
-      <c r="T82" s="253"/>
-      <c r="U82" s="253"/>
-      <c r="V82" s="253"/>
-      <c r="W82" s="253"/>
-      <c r="X82" s="253"/>
+      <c r="Q82" s="254"/>
+      <c r="R82" s="254"/>
+      <c r="S82" s="254"/>
+      <c r="T82" s="254"/>
+      <c r="U82" s="254"/>
+      <c r="V82" s="254"/>
+      <c r="W82" s="254"/>
+      <c r="X82" s="254"/>
       <c r="Y82" s="7"/>
       <c r="Z82" s="7"/>
       <c r="AA82" s="114"/>
@@ -24153,20 +24192,20 @@
     </row>
     <row r="83" spans="2:29" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="97"/>
-      <c r="C83" s="262"/>
-      <c r="D83" s="263"/>
-      <c r="E83" s="263"/>
-      <c r="F83" s="292"/>
-      <c r="G83" s="292"/>
-      <c r="H83" s="292"/>
-      <c r="I83" s="292"/>
-      <c r="J83" s="292"/>
-      <c r="K83" s="292"/>
-      <c r="L83" s="292"/>
-      <c r="M83" s="292"/>
-      <c r="N83" s="292"/>
-      <c r="O83" s="292"/>
-      <c r="P83" s="251" t="s">
+      <c r="C83" s="263"/>
+      <c r="D83" s="264"/>
+      <c r="E83" s="264"/>
+      <c r="F83" s="293"/>
+      <c r="G83" s="293"/>
+      <c r="H83" s="293"/>
+      <c r="I83" s="293"/>
+      <c r="J83" s="293"/>
+      <c r="K83" s="293"/>
+      <c r="L83" s="293"/>
+      <c r="M83" s="293"/>
+      <c r="N83" s="293"/>
+      <c r="O83" s="293"/>
+      <c r="P83" s="252" t="s">
         <v>35</v>
       </c>
       <c r="Q83" s="200"/>
@@ -24185,20 +24224,20 @@
     </row>
     <row r="84" spans="2:29" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="97"/>
-      <c r="C84" s="264"/>
-      <c r="D84" s="265"/>
-      <c r="E84" s="265"/>
-      <c r="F84" s="292"/>
-      <c r="G84" s="292"/>
-      <c r="H84" s="292"/>
-      <c r="I84" s="292"/>
-      <c r="J84" s="292"/>
-      <c r="K84" s="292"/>
-      <c r="L84" s="292"/>
-      <c r="M84" s="292"/>
-      <c r="N84" s="292"/>
-      <c r="O84" s="292"/>
-      <c r="P84" s="251" t="s">
+      <c r="C84" s="265"/>
+      <c r="D84" s="266"/>
+      <c r="E84" s="266"/>
+      <c r="F84" s="293"/>
+      <c r="G84" s="293"/>
+      <c r="H84" s="293"/>
+      <c r="I84" s="293"/>
+      <c r="J84" s="293"/>
+      <c r="K84" s="293"/>
+      <c r="L84" s="293"/>
+      <c r="M84" s="293"/>
+      <c r="N84" s="293"/>
+      <c r="O84" s="293"/>
+      <c r="P84" s="252" t="s">
         <v>33</v>
       </c>
       <c r="Q84" s="200"/>
@@ -24248,17 +24287,17 @@
     <row r="86" spans="2:29" s="6" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="97"/>
       <c r="C86" s="7"/>
-      <c r="D86" s="286" t="s">
+      <c r="D86" s="287" t="s">
         <v>33</v>
       </c>
-      <c r="E86" s="286"/>
+      <c r="E86" s="287"/>
       <c r="F86" s="54"/>
-      <c r="G86" s="277"/>
-      <c r="H86" s="278"/>
-      <c r="I86" s="278"/>
-      <c r="J86" s="278"/>
-      <c r="K86" s="278"/>
-      <c r="L86" s="279"/>
+      <c r="G86" s="278"/>
+      <c r="H86" s="279"/>
+      <c r="I86" s="279"/>
+      <c r="J86" s="279"/>
+      <c r="K86" s="279"/>
+      <c r="L86" s="280"/>
       <c r="M86" s="7"/>
       <c r="N86" s="88"/>
       <c r="O86" s="88"/>
@@ -24280,29 +24319,29 @@
     <row r="87" spans="2:29" s="6" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="97"/>
       <c r="C87" s="7"/>
-      <c r="D87" s="286"/>
-      <c r="E87" s="286"/>
+      <c r="D87" s="287"/>
+      <c r="E87" s="287"/>
       <c r="F87" s="54"/>
-      <c r="G87" s="280"/>
-      <c r="H87" s="281"/>
-      <c r="I87" s="281"/>
-      <c r="J87" s="281"/>
-      <c r="K87" s="281"/>
-      <c r="L87" s="282"/>
+      <c r="G87" s="281"/>
+      <c r="H87" s="282"/>
+      <c r="I87" s="282"/>
+      <c r="J87" s="282"/>
+      <c r="K87" s="282"/>
+      <c r="L87" s="283"/>
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
-      <c r="P87" s="254" t="s">
+      <c r="P87" s="255" t="s">
         <v>70</v>
       </c>
-      <c r="Q87" s="255"/>
-      <c r="R87" s="255"/>
-      <c r="S87" s="255"/>
-      <c r="T87" s="255"/>
-      <c r="U87" s="255"/>
-      <c r="V87" s="255"/>
-      <c r="W87" s="255"/>
-      <c r="X87" s="256"/>
+      <c r="Q87" s="256"/>
+      <c r="R87" s="256"/>
+      <c r="S87" s="256"/>
+      <c r="T87" s="256"/>
+      <c r="U87" s="256"/>
+      <c r="V87" s="256"/>
+      <c r="W87" s="256"/>
+      <c r="X87" s="257"/>
       <c r="Y87" s="45"/>
       <c r="Z87" s="45"/>
       <c r="AA87" s="104"/>
@@ -24312,27 +24351,27 @@
     <row r="88" spans="2:29" s="6" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="97"/>
       <c r="C88" s="7"/>
-      <c r="D88" s="286"/>
-      <c r="E88" s="286"/>
+      <c r="D88" s="287"/>
+      <c r="E88" s="287"/>
       <c r="F88" s="54"/>
-      <c r="G88" s="280"/>
-      <c r="H88" s="281"/>
-      <c r="I88" s="281"/>
-      <c r="J88" s="281"/>
-      <c r="K88" s="281"/>
-      <c r="L88" s="282"/>
+      <c r="G88" s="281"/>
+      <c r="H88" s="282"/>
+      <c r="I88" s="282"/>
+      <c r="J88" s="282"/>
+      <c r="K88" s="282"/>
+      <c r="L88" s="283"/>
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
-      <c r="P88" s="257"/>
-      <c r="Q88" s="258"/>
-      <c r="R88" s="258"/>
-      <c r="S88" s="258"/>
-      <c r="T88" s="258"/>
-      <c r="U88" s="258"/>
-      <c r="V88" s="258"/>
-      <c r="W88" s="258"/>
-      <c r="X88" s="259"/>
+      <c r="P88" s="258"/>
+      <c r="Q88" s="259"/>
+      <c r="R88" s="259"/>
+      <c r="S88" s="259"/>
+      <c r="T88" s="259"/>
+      <c r="U88" s="259"/>
+      <c r="V88" s="259"/>
+      <c r="W88" s="259"/>
+      <c r="X88" s="260"/>
       <c r="Y88" s="45"/>
       <c r="Z88" s="45"/>
       <c r="AA88" s="101"/>
@@ -24342,15 +24381,15 @@
     <row r="89" spans="2:29" s="6" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="97"/>
       <c r="C89" s="7"/>
-      <c r="D89" s="286"/>
-      <c r="E89" s="286"/>
+      <c r="D89" s="287"/>
+      <c r="E89" s="287"/>
       <c r="F89" s="54"/>
-      <c r="G89" s="280"/>
-      <c r="H89" s="281"/>
-      <c r="I89" s="281"/>
-      <c r="J89" s="281"/>
-      <c r="K89" s="281"/>
-      <c r="L89" s="282"/>
+      <c r="G89" s="281"/>
+      <c r="H89" s="282"/>
+      <c r="I89" s="282"/>
+      <c r="J89" s="282"/>
+      <c r="K89" s="282"/>
+      <c r="L89" s="283"/>
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
@@ -24371,30 +24410,30 @@
     <row r="90" spans="2:29" s="6" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="97"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="286"/>
-      <c r="E90" s="286"/>
+      <c r="D90" s="287"/>
+      <c r="E90" s="287"/>
       <c r="F90" s="54"/>
-      <c r="G90" s="283"/>
-      <c r="H90" s="284"/>
-      <c r="I90" s="284"/>
-      <c r="J90" s="284"/>
-      <c r="K90" s="284"/>
-      <c r="L90" s="285"/>
+      <c r="G90" s="284"/>
+      <c r="H90" s="285"/>
+      <c r="I90" s="285"/>
+      <c r="J90" s="285"/>
+      <c r="K90" s="285"/>
+      <c r="L90" s="286"/>
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
-      <c r="P90" s="274" t="s">
+      <c r="P90" s="275" t="s">
         <v>78</v>
       </c>
-      <c r="Q90" s="275"/>
-      <c r="R90" s="276"/>
+      <c r="Q90" s="276"/>
+      <c r="R90" s="277"/>
       <c r="S90" s="45"/>
-      <c r="T90" s="274" t="s">
+      <c r="T90" s="275" t="s">
         <v>71</v>
       </c>
-      <c r="U90" s="275"/>
-      <c r="V90" s="275"/>
-      <c r="W90" s="275"/>
-      <c r="X90" s="276"/>
+      <c r="U90" s="276"/>
+      <c r="V90" s="276"/>
+      <c r="W90" s="276"/>
+      <c r="X90" s="277"/>
       <c r="Y90" s="45"/>
       <c r="Z90" s="45"/>
       <c r="AA90" s="101"/>
@@ -24415,9 +24454,9 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
-      <c r="P91" s="246"/>
-      <c r="Q91" s="246"/>
-      <c r="R91" s="246"/>
+      <c r="P91" s="247"/>
+      <c r="Q91" s="247"/>
+      <c r="R91" s="247"/>
       <c r="S91" s="49"/>
       <c r="T91" s="127"/>
       <c r="U91" s="127"/>
@@ -24437,12 +24476,12 @@
       </c>
       <c r="E92" s="49"/>
       <c r="F92" s="49"/>
-      <c r="G92" s="247"/>
-      <c r="H92" s="247"/>
-      <c r="I92" s="247"/>
-      <c r="J92" s="247"/>
-      <c r="K92" s="247"/>
-      <c r="L92" s="247"/>
+      <c r="G92" s="248"/>
+      <c r="H92" s="248"/>
+      <c r="I92" s="248"/>
+      <c r="J92" s="248"/>
+      <c r="K92" s="248"/>
+      <c r="L92" s="248"/>
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
@@ -24468,20 +24507,20 @@
       </c>
       <c r="E93" s="49"/>
       <c r="F93" s="49"/>
-      <c r="G93" s="289"/>
-      <c r="H93" s="289"/>
-      <c r="I93" s="289"/>
-      <c r="J93" s="289"/>
-      <c r="K93" s="289"/>
-      <c r="L93" s="289"/>
+      <c r="G93" s="290"/>
+      <c r="H93" s="290"/>
+      <c r="I93" s="290"/>
+      <c r="J93" s="290"/>
+      <c r="K93" s="290"/>
+      <c r="L93" s="290"/>
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
-      <c r="P93" s="287" t="s">
+      <c r="P93" s="288" t="s">
         <v>79</v>
       </c>
-      <c r="Q93" s="287"/>
-      <c r="R93" s="287"/>
+      <c r="Q93" s="288"/>
+      <c r="R93" s="288"/>
       <c r="S93" s="27"/>
       <c r="T93" s="27"/>
       <c r="U93" s="27"/>
@@ -24501,18 +24540,18 @@
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
-      <c r="G94" s="288"/>
-      <c r="H94" s="288"/>
-      <c r="I94" s="288"/>
-      <c r="J94" s="288"/>
-      <c r="K94" s="288"/>
-      <c r="L94" s="288"/>
+      <c r="G94" s="289"/>
+      <c r="H94" s="289"/>
+      <c r="I94" s="289"/>
+      <c r="J94" s="289"/>
+      <c r="K94" s="289"/>
+      <c r="L94" s="289"/>
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
-      <c r="P94" s="287"/>
-      <c r="Q94" s="287"/>
-      <c r="R94" s="287"/>
+      <c r="P94" s="288"/>
+      <c r="Q94" s="288"/>
+      <c r="R94" s="288"/>
       <c r="S94" s="27"/>
       <c r="T94" s="27"/>
       <c r="U94" s="27"/>
@@ -24527,10 +24566,10 @@
     <row r="95" spans="2:29" s="6" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B95" s="97"/>
       <c r="C95" s="7"/>
-      <c r="D95" s="245" t="s">
+      <c r="D95" s="246" t="s">
         <v>102</v>
       </c>
-      <c r="E95" s="245"/>
+      <c r="E95" s="246"/>
       <c r="F95" s="48"/>
       <c r="G95" s="203"/>
       <c r="H95" s="203"/>
@@ -24543,9 +24582,9 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
-      <c r="P95" s="290"/>
-      <c r="Q95" s="290"/>
-      <c r="R95" s="290"/>
+      <c r="P95" s="291"/>
+      <c r="Q95" s="291"/>
+      <c r="R95" s="291"/>
       <c r="S95" s="27"/>
       <c r="T95" s="27"/>
       <c r="U95" s="27"/>
@@ -24571,19 +24610,19 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
-      <c r="P96" s="248" t="s">
+      <c r="P96" s="249" t="s">
         <v>107</v>
       </c>
-      <c r="Q96" s="249"/>
-      <c r="R96" s="250"/>
-      <c r="S96" s="272"/>
-      <c r="T96" s="248" t="s">
+      <c r="Q96" s="250"/>
+      <c r="R96" s="251"/>
+      <c r="S96" s="273"/>
+      <c r="T96" s="249" t="s">
         <v>107</v>
       </c>
-      <c r="U96" s="249"/>
-      <c r="V96" s="249"/>
-      <c r="W96" s="249"/>
-      <c r="X96" s="250"/>
+      <c r="U96" s="250"/>
+      <c r="V96" s="250"/>
+      <c r="W96" s="250"/>
+      <c r="X96" s="251"/>
       <c r="Y96" s="40"/>
       <c r="Z96" s="40"/>
       <c r="AA96" s="104"/>
@@ -24611,14 +24650,14 @@
       </c>
       <c r="Q97" s="43"/>
       <c r="R97" s="131"/>
-      <c r="S97" s="273"/>
-      <c r="T97" s="266" t="s">
+      <c r="S97" s="274"/>
+      <c r="T97" s="267" t="s">
         <v>35</v>
       </c>
-      <c r="U97" s="267"/>
-      <c r="V97" s="267"/>
-      <c r="W97" s="267"/>
-      <c r="X97" s="268"/>
+      <c r="U97" s="268"/>
+      <c r="V97" s="268"/>
+      <c r="W97" s="268"/>
+      <c r="X97" s="269"/>
       <c r="Y97" s="7"/>
       <c r="Z97" s="7"/>
       <c r="AA97" s="104"/>
@@ -24644,14 +24683,14 @@
       </c>
       <c r="Q98" s="43"/>
       <c r="R98" s="43"/>
-      <c r="S98" s="273"/>
-      <c r="T98" s="269" t="s">
+      <c r="S98" s="274"/>
+      <c r="T98" s="270" t="s">
         <v>36</v>
       </c>
-      <c r="U98" s="270"/>
-      <c r="V98" s="270"/>
-      <c r="W98" s="270"/>
-      <c r="X98" s="271"/>
+      <c r="U98" s="271"/>
+      <c r="V98" s="271"/>
+      <c r="W98" s="271"/>
+      <c r="X98" s="272"/>
       <c r="Y98" s="7"/>
       <c r="Z98" s="7"/>
       <c r="AA98" s="104"/>

</xml_diff>